<commit_message>
Added Extent Report Feature
</commit_message>
<xml_diff>
--- a/src/main/java/com/yocket/testData/YocketMastersTestData.xlsx
+++ b/src/main/java/com/yocket/testData/YocketMastersTestData.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/872903_cognizant_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{08456A84-0F8B-40C7-A7AE-0E62D04977CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A83AA37-9926-4378-9FC3-BBB54B62E5D1}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="8_{08456A84-0F8B-40C7-A7AE-0E62D04977CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FE082C7-3C53-4187-879A-380642AD354F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{6B2FEF9C-0EFF-48BA-B121-656732A5C18E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{6B2FEF9C-0EFF-48BA-B121-656732A5C18E}"/>
   </bookViews>
   <sheets>
     <sheet name="mastersDetails" sheetId="1" r:id="rId1"/>
-    <sheet name="invalidCountryandCourse" sheetId="3" r:id="rId2"/>
-    <sheet name="invalidCollegeMajorGPA" sheetId="4" r:id="rId3"/>
+    <sheet name="invalidCountry" sheetId="5" r:id="rId2"/>
+    <sheet name="invalidCourse" sheetId="3" r:id="rId3"/>
+    <sheet name="invalidCollege" sheetId="7" r:id="rId4"/>
+    <sheet name="invalidMajor" sheetId="6" r:id="rId5"/>
+    <sheet name="invalidGPA" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="18">
   <si>
     <t xml:space="preserve">Country </t>
   </si>
@@ -80,16 +83,16 @@
     <t>*$&amp;</t>
   </si>
   <si>
-    <t>&amp;%*</t>
-  </si>
-  <si>
-    <t>*$%&amp;</t>
-  </si>
-  <si>
-    <t>hks</t>
-  </si>
-  <si>
-    <t>*#^</t>
+    <t>iwm</t>
+  </si>
+  <si>
+    <t>*^%(</t>
+  </si>
+  <si>
+    <t>*^$(</t>
+  </si>
+  <si>
+    <t>&amp;$%*</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -542,11 +545,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DED298B-AB72-4DE4-BBDE-E870F6E51019}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AB3EB5-9750-45C0-818B-7A6DCE43E0AB}">
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DED298B-AB72-4DE4-BBDE-E870F6E51019}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -564,165 +603,263 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>653</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2">
+        <v>39421</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2">
-        <v>39421</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5ACFE0-F879-4B37-B62D-3FC8C450A657}">
-  <dimension ref="A1:C10"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93959E16-A746-4050-8B83-18CEC76223A6}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{481B6E19-2CBE-4B12-9626-655B556D915A}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>9834</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5ACFE0-F879-4B37-B62D-3FC8C450A657}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>123</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
-        <v>5431</v>
-      </c>
-      <c r="C5">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
+      <c r="E5">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>